<commit_message>
modifiche ai nomi delle stazioni dei pullman
</commit_message>
<xml_diff>
--- a/Java/BGTransport/src/main/resources/excel/list/pullman_stop_list.xlsx
+++ b/Java/BGTransport/src/main/resources/excel/list/pullman_stop_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e2a8a40ee8ef1bb/Desktop/BGLocalTransport/BGTransports/Java/BGTransport/src/main/resources/excel/list/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/86d5980519d90a03/Desktop/BGTransports/Java/BGTransport/src/main/resources/excel/list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{F52A1665-4A96-4E8E-9E70-37CF0E18A79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25EC4E36-CAED-49E9-9BD6-B65DEC772EC0}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{F52A1665-4A96-4E8E-9E70-37CF0E18A79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8897CFF9-961A-4CB8-839E-5B7D2C3D4662}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{C5C4A483-4445-4EA3-8165-95B06087C953}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C5C4A483-4445-4EA3-8165-95B06087C953}"/>
   </bookViews>
   <sheets>
     <sheet name="Fermate" sheetId="2" r:id="rId1"/>
@@ -4140,9 +4140,6 @@
     <t>via Petrarca fr.12/14 Banca d Italia</t>
   </si>
   <si>
-    <t>via Presolana Centro per l impiego</t>
-  </si>
-  <si>
     <t>via Ruggeri da Stabello 1</t>
   </si>
   <si>
@@ -5680,6 +5677,9 @@
   </si>
   <si>
     <t>9.658735</t>
+  </si>
+  <si>
+    <t>via Presolana Centro per l'impiego</t>
   </si>
 </sst>
 </file>
@@ -6931,10 +6931,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7447,12 +7443,12 @@
   <dimension ref="A1:H289"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="49.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" style="23" bestFit="1" customWidth="1"/>
@@ -7461,19 +7457,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
+        <v>627</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>628</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C1" s="17" t="s">
         <v>629</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="21" t="s">
         <v>630</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>631</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -7487,10 +7483,10 @@
         <v>305</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -7504,10 +7500,10 @@
         <v>305</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -7521,10 +7517,10 @@
         <v>305</v>
       </c>
       <c r="D4" s="19" t="s">
+        <v>632</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>633</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -7538,10 +7534,10 @@
         <v>305</v>
       </c>
       <c r="D5" s="20" t="s">
+        <v>634</v>
+      </c>
+      <c r="E5" s="20" t="s">
         <v>635</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -7555,10 +7551,10 @@
         <v>305</v>
       </c>
       <c r="D6" s="19" t="s">
+        <v>636</v>
+      </c>
+      <c r="E6" s="19" t="s">
         <v>637</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>638</v>
       </c>
       <c r="H6" s="25"/>
     </row>
@@ -7573,10 +7569,10 @@
         <v>305</v>
       </c>
       <c r="D7" s="20" t="s">
+        <v>638</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>639</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -7590,10 +7586,10 @@
         <v>305</v>
       </c>
       <c r="D8" s="19" t="s">
+        <v>640</v>
+      </c>
+      <c r="E8" s="19" t="s">
         <v>641</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -7607,10 +7603,10 @@
         <v>305</v>
       </c>
       <c r="D9" s="20" t="s">
+        <v>642</v>
+      </c>
+      <c r="E9" s="20" t="s">
         <v>643</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -7624,10 +7620,10 @@
         <v>305</v>
       </c>
       <c r="D10" s="19" t="s">
+        <v>644</v>
+      </c>
+      <c r="E10" s="19" t="s">
         <v>645</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -7641,10 +7637,10 @@
         <v>305</v>
       </c>
       <c r="D11" s="20" t="s">
+        <v>646</v>
+      </c>
+      <c r="E11" s="20" t="s">
         <v>647</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -7658,10 +7654,10 @@
         <v>305</v>
       </c>
       <c r="D12" s="19" t="s">
+        <v>648</v>
+      </c>
+      <c r="E12" s="19" t="s">
         <v>649</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -7675,10 +7671,10 @@
         <v>305</v>
       </c>
       <c r="D13" s="20" t="s">
+        <v>650</v>
+      </c>
+      <c r="E13" s="20" t="s">
         <v>651</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -7692,10 +7688,10 @@
         <v>305</v>
       </c>
       <c r="D14" s="19" t="s">
+        <v>652</v>
+      </c>
+      <c r="E14" s="19" t="s">
         <v>653</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -7709,10 +7705,10 @@
         <v>305</v>
       </c>
       <c r="D15" s="20" t="s">
+        <v>654</v>
+      </c>
+      <c r="E15" s="20" t="s">
         <v>655</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -7726,10 +7722,10 @@
         <v>305</v>
       </c>
       <c r="D16" s="19" t="s">
+        <v>652</v>
+      </c>
+      <c r="E16" s="19" t="s">
         <v>653</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -7743,10 +7739,10 @@
         <v>305</v>
       </c>
       <c r="D17" s="20" t="s">
+        <v>652</v>
+      </c>
+      <c r="E17" s="20" t="s">
         <v>653</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -7760,10 +7756,10 @@
         <v>305</v>
       </c>
       <c r="D18" s="19" t="s">
+        <v>654</v>
+      </c>
+      <c r="E18" s="19" t="s">
         <v>655</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -7777,10 +7773,10 @@
         <v>305</v>
       </c>
       <c r="D19" s="20" t="s">
+        <v>654</v>
+      </c>
+      <c r="E19" s="20" t="s">
         <v>655</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -7794,10 +7790,10 @@
         <v>305</v>
       </c>
       <c r="D20" s="19" t="s">
+        <v>654</v>
+      </c>
+      <c r="E20" s="19" t="s">
         <v>655</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -7811,10 +7807,10 @@
         <v>305</v>
       </c>
       <c r="D21" s="20" t="s">
+        <v>654</v>
+      </c>
+      <c r="E21" s="20" t="s">
         <v>655</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -7828,10 +7824,10 @@
         <v>305</v>
       </c>
       <c r="D22" s="19" t="s">
+        <v>654</v>
+      </c>
+      <c r="E22" s="19" t="s">
         <v>655</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -7845,10 +7841,10 @@
         <v>305</v>
       </c>
       <c r="D23" s="20" t="s">
+        <v>654</v>
+      </c>
+      <c r="E23" s="20" t="s">
         <v>655</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -7862,10 +7858,10 @@
         <v>305</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -7879,10 +7875,10 @@
         <v>305</v>
       </c>
       <c r="D25" s="20" t="s">
+        <v>656</v>
+      </c>
+      <c r="E25" s="20" t="s">
         <v>657</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>658</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -7896,10 +7892,10 @@
         <v>305</v>
       </c>
       <c r="D26" s="19" t="s">
+        <v>658</v>
+      </c>
+      <c r="E26" s="19" t="s">
         <v>659</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -7913,10 +7909,10 @@
         <v>305</v>
       </c>
       <c r="D27" s="20" t="s">
+        <v>660</v>
+      </c>
+      <c r="E27" s="20" t="s">
         <v>661</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -7930,10 +7926,10 @@
         <v>305</v>
       </c>
       <c r="D28" s="19" t="s">
+        <v>662</v>
+      </c>
+      <c r="E28" s="19" t="s">
         <v>663</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -7947,10 +7943,10 @@
         <v>305</v>
       </c>
       <c r="D29" s="20" t="s">
+        <v>664</v>
+      </c>
+      <c r="E29" s="20" t="s">
         <v>665</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -7964,10 +7960,10 @@
         <v>305</v>
       </c>
       <c r="D30" s="19" t="s">
+        <v>666</v>
+      </c>
+      <c r="E30" s="19" t="s">
         <v>667</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -7981,10 +7977,10 @@
         <v>305</v>
       </c>
       <c r="D31" s="20" t="s">
+        <v>668</v>
+      </c>
+      <c r="E31" s="20" t="s">
         <v>669</v>
-      </c>
-      <c r="E31" s="20" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -7998,10 +7994,10 @@
         <v>305</v>
       </c>
       <c r="D32" s="19" t="s">
+        <v>670</v>
+      </c>
+      <c r="E32" s="19" t="s">
         <v>671</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -8015,10 +8011,10 @@
         <v>305</v>
       </c>
       <c r="D33" s="20" t="s">
+        <v>672</v>
+      </c>
+      <c r="E33" s="20" t="s">
         <v>673</v>
-      </c>
-      <c r="E33" s="20" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -8032,10 +8028,10 @@
         <v>305</v>
       </c>
       <c r="D34" s="19" t="s">
+        <v>674</v>
+      </c>
+      <c r="E34" s="19" t="s">
         <v>675</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -8049,10 +8045,10 @@
         <v>305</v>
       </c>
       <c r="D35" s="20" t="s">
+        <v>676</v>
+      </c>
+      <c r="E35" s="20" t="s">
         <v>677</v>
-      </c>
-      <c r="E35" s="20" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -8066,10 +8062,10 @@
         <v>305</v>
       </c>
       <c r="D36" s="19" t="s">
+        <v>678</v>
+      </c>
+      <c r="E36" s="19" t="s">
         <v>679</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -8083,10 +8079,10 @@
         <v>305</v>
       </c>
       <c r="D37" s="20" t="s">
+        <v>680</v>
+      </c>
+      <c r="E37" s="20" t="s">
         <v>681</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -8100,10 +8096,10 @@
         <v>305</v>
       </c>
       <c r="D38" s="19" t="s">
+        <v>682</v>
+      </c>
+      <c r="E38" s="19" t="s">
         <v>683</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -8117,10 +8113,10 @@
         <v>305</v>
       </c>
       <c r="D39" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="E39" s="20" t="s">
         <v>685</v>
-      </c>
-      <c r="E39" s="20" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -8134,10 +8130,10 @@
         <v>305</v>
       </c>
       <c r="D40" s="19" t="s">
+        <v>686</v>
+      </c>
+      <c r="E40" s="19" t="s">
         <v>687</v>
-      </c>
-      <c r="E40" s="19" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -8151,10 +8147,10 @@
         <v>305</v>
       </c>
       <c r="D41" s="20" t="s">
+        <v>688</v>
+      </c>
+      <c r="E41" s="20" t="s">
         <v>689</v>
-      </c>
-      <c r="E41" s="20" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -8168,10 +8164,10 @@
         <v>305</v>
       </c>
       <c r="D42" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="E42" s="19" t="s">
         <v>689</v>
-      </c>
-      <c r="E42" s="19" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -8185,10 +8181,10 @@
         <v>305</v>
       </c>
       <c r="D43" s="20" t="s">
+        <v>690</v>
+      </c>
+      <c r="E43" s="20" t="s">
         <v>691</v>
-      </c>
-      <c r="E43" s="20" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -8202,10 +8198,10 @@
         <v>305</v>
       </c>
       <c r="D44" s="19" t="s">
+        <v>692</v>
+      </c>
+      <c r="E44" s="19" t="s">
         <v>693</v>
-      </c>
-      <c r="E44" s="19" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -8219,10 +8215,10 @@
         <v>305</v>
       </c>
       <c r="D45" s="20" t="s">
+        <v>694</v>
+      </c>
+      <c r="E45" s="20" t="s">
         <v>695</v>
-      </c>
-      <c r="E45" s="20" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -8236,10 +8232,10 @@
         <v>305</v>
       </c>
       <c r="D46" s="19" t="s">
+        <v>696</v>
+      </c>
+      <c r="E46" s="19" t="s">
         <v>697</v>
-      </c>
-      <c r="E46" s="19" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -8253,10 +8249,10 @@
         <v>305</v>
       </c>
       <c r="D47" s="20" t="s">
+        <v>698</v>
+      </c>
+      <c r="E47" s="20" t="s">
         <v>699</v>
-      </c>
-      <c r="E47" s="20" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -8270,10 +8266,10 @@
         <v>305</v>
       </c>
       <c r="D48" s="19" t="s">
+        <v>700</v>
+      </c>
+      <c r="E48" s="19" t="s">
         <v>701</v>
-      </c>
-      <c r="E48" s="19" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -8287,10 +8283,10 @@
         <v>305</v>
       </c>
       <c r="D49" s="20" t="s">
+        <v>702</v>
+      </c>
+      <c r="E49" s="20" t="s">
         <v>703</v>
-      </c>
-      <c r="E49" s="20" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -8304,10 +8300,10 @@
         <v>305</v>
       </c>
       <c r="D50" s="19" t="s">
+        <v>704</v>
+      </c>
+      <c r="E50" s="19" t="s">
         <v>705</v>
-      </c>
-      <c r="E50" s="19" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -8321,10 +8317,10 @@
         <v>305</v>
       </c>
       <c r="D51" s="20" t="s">
+        <v>706</v>
+      </c>
+      <c r="E51" s="20" t="s">
         <v>707</v>
-      </c>
-      <c r="E51" s="20" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -8338,10 +8334,10 @@
         <v>305</v>
       </c>
       <c r="D52" s="19" t="s">
+        <v>708</v>
+      </c>
+      <c r="E52" s="19" t="s">
         <v>709</v>
-      </c>
-      <c r="E52" s="19" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -8355,10 +8351,10 @@
         <v>305</v>
       </c>
       <c r="D53" s="20" t="s">
+        <v>710</v>
+      </c>
+      <c r="E53" s="20" t="s">
         <v>711</v>
-      </c>
-      <c r="E53" s="20" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -8372,10 +8368,10 @@
         <v>305</v>
       </c>
       <c r="D54" s="19" t="s">
+        <v>712</v>
+      </c>
+      <c r="E54" s="19" t="s">
         <v>713</v>
-      </c>
-      <c r="E54" s="19" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -8389,10 +8385,10 @@
         <v>305</v>
       </c>
       <c r="D55" s="20" t="s">
+        <v>714</v>
+      </c>
+      <c r="E55" s="20" t="s">
         <v>715</v>
-      </c>
-      <c r="E55" s="20" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -8406,10 +8402,10 @@
         <v>305</v>
       </c>
       <c r="D56" s="19" t="s">
+        <v>716</v>
+      </c>
+      <c r="E56" s="19" t="s">
         <v>717</v>
-      </c>
-      <c r="E56" s="19" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -8423,10 +8419,10 @@
         <v>305</v>
       </c>
       <c r="D57" s="20" t="s">
+        <v>718</v>
+      </c>
+      <c r="E57" s="20" t="s">
         <v>719</v>
-      </c>
-      <c r="E57" s="20" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -8440,10 +8436,10 @@
         <v>305</v>
       </c>
       <c r="D58" s="19" t="s">
+        <v>720</v>
+      </c>
+      <c r="E58" s="19" t="s">
         <v>721</v>
-      </c>
-      <c r="E58" s="19" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -8457,10 +8453,10 @@
         <v>305</v>
       </c>
       <c r="D59" s="20" t="s">
+        <v>716</v>
+      </c>
+      <c r="E59" s="20" t="s">
         <v>717</v>
-      </c>
-      <c r="E59" s="20" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -8474,10 +8470,10 @@
         <v>305</v>
       </c>
       <c r="D60" s="19" t="s">
+        <v>722</v>
+      </c>
+      <c r="E60" s="19" t="s">
         <v>723</v>
-      </c>
-      <c r="E60" s="19" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -8491,10 +8487,10 @@
         <v>305</v>
       </c>
       <c r="D61" s="20" t="s">
+        <v>724</v>
+      </c>
+      <c r="E61" s="20" t="s">
         <v>725</v>
-      </c>
-      <c r="E61" s="20" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -8508,10 +8504,10 @@
         <v>305</v>
       </c>
       <c r="D62" s="19" t="s">
+        <v>726</v>
+      </c>
+      <c r="E62" s="19" t="s">
         <v>727</v>
-      </c>
-      <c r="E62" s="19" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -8525,10 +8521,10 @@
         <v>305</v>
       </c>
       <c r="D63" s="20" t="s">
+        <v>728</v>
+      </c>
+      <c r="E63" s="20" t="s">
         <v>729</v>
-      </c>
-      <c r="E63" s="20" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -8542,10 +8538,10 @@
         <v>305</v>
       </c>
       <c r="D64" s="19" t="s">
+        <v>730</v>
+      </c>
+      <c r="E64" s="19" t="s">
         <v>731</v>
-      </c>
-      <c r="E64" s="19" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -8559,10 +8555,10 @@
         <v>305</v>
       </c>
       <c r="D65" s="20" t="s">
+        <v>732</v>
+      </c>
+      <c r="E65" s="20" t="s">
         <v>733</v>
-      </c>
-      <c r="E65" s="20" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -8576,10 +8572,10 @@
         <v>305</v>
       </c>
       <c r="D66" s="19" t="s">
+        <v>734</v>
+      </c>
+      <c r="E66" s="19" t="s">
         <v>735</v>
-      </c>
-      <c r="E66" s="19" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -8593,10 +8589,10 @@
         <v>305</v>
       </c>
       <c r="D67" s="20" t="s">
+        <v>736</v>
+      </c>
+      <c r="E67" s="20" t="s">
         <v>737</v>
-      </c>
-      <c r="E67" s="20" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -8610,10 +8606,10 @@
         <v>305</v>
       </c>
       <c r="D68" s="19" t="s">
+        <v>738</v>
+      </c>
+      <c r="E68" s="19" t="s">
         <v>739</v>
-      </c>
-      <c r="E68" s="19" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -8627,10 +8623,10 @@
         <v>305</v>
       </c>
       <c r="D69" s="20" t="s">
+        <v>740</v>
+      </c>
+      <c r="E69" s="20" t="s">
         <v>741</v>
-      </c>
-      <c r="E69" s="20" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -8644,10 +8640,10 @@
         <v>305</v>
       </c>
       <c r="D70" s="19" t="s">
+        <v>742</v>
+      </c>
+      <c r="E70" s="19" t="s">
         <v>743</v>
-      </c>
-      <c r="E70" s="19" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -8661,10 +8657,10 @@
         <v>305</v>
       </c>
       <c r="D71" s="20" t="s">
+        <v>744</v>
+      </c>
+      <c r="E71" s="20" t="s">
         <v>745</v>
-      </c>
-      <c r="E71" s="20" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -8678,10 +8674,10 @@
         <v>305</v>
       </c>
       <c r="D72" s="19" t="s">
+        <v>746</v>
+      </c>
+      <c r="E72" s="19" t="s">
         <v>747</v>
-      </c>
-      <c r="E72" s="19" t="s">
-        <v>748</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -8695,10 +8691,10 @@
         <v>305</v>
       </c>
       <c r="D73" s="20" t="s">
+        <v>748</v>
+      </c>
+      <c r="E73" s="20" t="s">
         <v>749</v>
-      </c>
-      <c r="E73" s="20" t="s">
-        <v>750</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -8712,10 +8708,10 @@
         <v>305</v>
       </c>
       <c r="D74" s="19" t="s">
+        <v>750</v>
+      </c>
+      <c r="E74" s="19" t="s">
         <v>751</v>
-      </c>
-      <c r="E74" s="19" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -8729,10 +8725,10 @@
         <v>305</v>
       </c>
       <c r="D75" s="20" t="s">
+        <v>752</v>
+      </c>
+      <c r="E75" s="20" t="s">
         <v>753</v>
-      </c>
-      <c r="E75" s="20" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -8746,10 +8742,10 @@
         <v>305</v>
       </c>
       <c r="D76" s="19" t="s">
+        <v>754</v>
+      </c>
+      <c r="E76" s="19" t="s">
         <v>755</v>
-      </c>
-      <c r="E76" s="19" t="s">
-        <v>756</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -8763,10 +8759,10 @@
         <v>305</v>
       </c>
       <c r="D77" s="20" t="s">
+        <v>756</v>
+      </c>
+      <c r="E77" s="20" t="s">
         <v>757</v>
-      </c>
-      <c r="E77" s="20" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -8780,10 +8776,10 @@
         <v>305</v>
       </c>
       <c r="D78" s="19" t="s">
+        <v>758</v>
+      </c>
+      <c r="E78" s="19" t="s">
         <v>759</v>
-      </c>
-      <c r="E78" s="19" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -8797,10 +8793,10 @@
         <v>305</v>
       </c>
       <c r="D79" s="20" t="s">
+        <v>760</v>
+      </c>
+      <c r="E79" s="20" t="s">
         <v>761</v>
-      </c>
-      <c r="E79" s="20" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -8814,10 +8810,10 @@
         <v>305</v>
       </c>
       <c r="D80" s="19" t="s">
+        <v>762</v>
+      </c>
+      <c r="E80" s="19" t="s">
         <v>763</v>
-      </c>
-      <c r="E80" s="19" t="s">
-        <v>764</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -8831,10 +8827,10 @@
         <v>305</v>
       </c>
       <c r="D81" s="20" t="s">
+        <v>760</v>
+      </c>
+      <c r="E81" s="20" t="s">
         <v>761</v>
-      </c>
-      <c r="E81" s="20" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -8848,10 +8844,10 @@
         <v>305</v>
       </c>
       <c r="D82" s="19" t="s">
+        <v>764</v>
+      </c>
+      <c r="E82" s="19" t="s">
         <v>765</v>
-      </c>
-      <c r="E82" s="19" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -8865,10 +8861,10 @@
         <v>305</v>
       </c>
       <c r="D83" s="20" t="s">
+        <v>766</v>
+      </c>
+      <c r="E83" s="20" t="s">
         <v>767</v>
-      </c>
-      <c r="E83" s="20" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -8882,10 +8878,10 @@
         <v>305</v>
       </c>
       <c r="D84" s="19" t="s">
+        <v>768</v>
+      </c>
+      <c r="E84" s="19" t="s">
         <v>769</v>
-      </c>
-      <c r="E84" s="19" t="s">
-        <v>770</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -8899,10 +8895,10 @@
         <v>305</v>
       </c>
       <c r="D85" s="20" t="s">
+        <v>770</v>
+      </c>
+      <c r="E85" s="20" t="s">
         <v>771</v>
-      </c>
-      <c r="E85" s="20" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -8916,10 +8912,10 @@
         <v>305</v>
       </c>
       <c r="D86" s="19" t="s">
+        <v>772</v>
+      </c>
+      <c r="E86" s="19" t="s">
         <v>773</v>
-      </c>
-      <c r="E86" s="19" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -8933,10 +8929,10 @@
         <v>305</v>
       </c>
       <c r="D87" s="20" t="s">
+        <v>774</v>
+      </c>
+      <c r="E87" s="20" t="s">
         <v>775</v>
-      </c>
-      <c r="E87" s="20" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -8950,10 +8946,10 @@
         <v>305</v>
       </c>
       <c r="D88" s="19" t="s">
+        <v>776</v>
+      </c>
+      <c r="E88" s="19" t="s">
         <v>777</v>
-      </c>
-      <c r="E88" s="19" t="s">
-        <v>778</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -8967,10 +8963,10 @@
         <v>305</v>
       </c>
       <c r="D89" s="20" t="s">
+        <v>778</v>
+      </c>
+      <c r="E89" s="20" t="s">
         <v>779</v>
-      </c>
-      <c r="E89" s="20" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -8984,10 +8980,10 @@
         <v>305</v>
       </c>
       <c r="D90" s="19" t="s">
+        <v>780</v>
+      </c>
+      <c r="E90" s="19" t="s">
         <v>781</v>
-      </c>
-      <c r="E90" s="19" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -9001,10 +8997,10 @@
         <v>305</v>
       </c>
       <c r="D91" s="20" t="s">
+        <v>782</v>
+      </c>
+      <c r="E91" s="20" t="s">
         <v>783</v>
-      </c>
-      <c r="E91" s="20" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -9018,10 +9014,10 @@
         <v>305</v>
       </c>
       <c r="D92" s="19" t="s">
+        <v>784</v>
+      </c>
+      <c r="E92" s="19" t="s">
         <v>785</v>
-      </c>
-      <c r="E92" s="19" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -9035,10 +9031,10 @@
         <v>305</v>
       </c>
       <c r="D93" s="20" t="s">
+        <v>672</v>
+      </c>
+      <c r="E93" s="20" t="s">
         <v>673</v>
-      </c>
-      <c r="E93" s="20" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -9052,10 +9048,10 @@
         <v>305</v>
       </c>
       <c r="D94" s="19" t="s">
+        <v>786</v>
+      </c>
+      <c r="E94" s="19" t="s">
         <v>787</v>
-      </c>
-      <c r="E94" s="19" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -9069,10 +9065,10 @@
         <v>305</v>
       </c>
       <c r="D95" s="20" t="s">
+        <v>788</v>
+      </c>
+      <c r="E95" s="20" t="s">
         <v>789</v>
-      </c>
-      <c r="E95" s="20" t="s">
-        <v>790</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -9086,10 +9082,10 @@
         <v>305</v>
       </c>
       <c r="D96" s="19" t="s">
+        <v>790</v>
+      </c>
+      <c r="E96" s="19" t="s">
         <v>791</v>
-      </c>
-      <c r="E96" s="19" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -9103,10 +9099,10 @@
         <v>305</v>
       </c>
       <c r="D97" s="20" t="s">
+        <v>792</v>
+      </c>
+      <c r="E97" s="20" t="s">
         <v>793</v>
-      </c>
-      <c r="E97" s="20" t="s">
-        <v>794</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -9120,10 +9116,10 @@
         <v>305</v>
       </c>
       <c r="D98" s="19" t="s">
+        <v>794</v>
+      </c>
+      <c r="E98" s="19" t="s">
         <v>795</v>
-      </c>
-      <c r="E98" s="19" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -9137,10 +9133,10 @@
         <v>305</v>
       </c>
       <c r="D99" s="20" t="s">
+        <v>796</v>
+      </c>
+      <c r="E99" s="20" t="s">
         <v>797</v>
-      </c>
-      <c r="E99" s="20" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -9154,10 +9150,10 @@
         <v>305</v>
       </c>
       <c r="D100" s="19" t="s">
+        <v>798</v>
+      </c>
+      <c r="E100" s="19" t="s">
         <v>799</v>
-      </c>
-      <c r="E100" s="19" t="s">
-        <v>800</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -9171,10 +9167,10 @@
         <v>305</v>
       </c>
       <c r="D101" s="20" t="s">
+        <v>800</v>
+      </c>
+      <c r="E101" s="20" t="s">
         <v>801</v>
-      </c>
-      <c r="E101" s="20" t="s">
-        <v>802</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -9188,10 +9184,10 @@
         <v>305</v>
       </c>
       <c r="D102" s="19" t="s">
+        <v>802</v>
+      </c>
+      <c r="E102" s="19" t="s">
         <v>803</v>
-      </c>
-      <c r="E102" s="19" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -9205,10 +9201,10 @@
         <v>305</v>
       </c>
       <c r="D103" s="20" t="s">
+        <v>804</v>
+      </c>
+      <c r="E103" s="20" t="s">
         <v>805</v>
-      </c>
-      <c r="E103" s="20" t="s">
-        <v>806</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -9222,10 +9218,10 @@
         <v>305</v>
       </c>
       <c r="D104" s="19" t="s">
+        <v>806</v>
+      </c>
+      <c r="E104" s="19" t="s">
         <v>807</v>
-      </c>
-      <c r="E104" s="19" t="s">
-        <v>808</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -9239,10 +9235,10 @@
         <v>305</v>
       </c>
       <c r="D105" s="20" t="s">
+        <v>808</v>
+      </c>
+      <c r="E105" s="20" t="s">
         <v>809</v>
-      </c>
-      <c r="E105" s="20" t="s">
-        <v>810</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -9256,10 +9252,10 @@
         <v>305</v>
       </c>
       <c r="D106" s="19" t="s">
+        <v>810</v>
+      </c>
+      <c r="E106" s="19" t="s">
         <v>811</v>
-      </c>
-      <c r="E106" s="19" t="s">
-        <v>812</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -9273,10 +9269,10 @@
         <v>305</v>
       </c>
       <c r="D107" s="20" t="s">
+        <v>812</v>
+      </c>
+      <c r="E107" s="20" t="s">
         <v>813</v>
-      </c>
-      <c r="E107" s="20" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -9290,10 +9286,10 @@
         <v>305</v>
       </c>
       <c r="D108" s="19" t="s">
+        <v>814</v>
+      </c>
+      <c r="E108" s="19" t="s">
         <v>815</v>
-      </c>
-      <c r="E108" s="19" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -9307,10 +9303,10 @@
         <v>305</v>
       </c>
       <c r="D109" s="20" t="s">
+        <v>816</v>
+      </c>
+      <c r="E109" s="20" t="s">
         <v>817</v>
-      </c>
-      <c r="E109" s="20" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -9324,10 +9320,10 @@
         <v>305</v>
       </c>
       <c r="D110" s="19" t="s">
+        <v>818</v>
+      </c>
+      <c r="E110" s="19" t="s">
         <v>819</v>
-      </c>
-      <c r="E110" s="19" t="s">
-        <v>820</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -9341,10 +9337,10 @@
         <v>305</v>
       </c>
       <c r="D111" s="20" t="s">
+        <v>820</v>
+      </c>
+      <c r="E111" s="20" t="s">
         <v>821</v>
-      </c>
-      <c r="E111" s="20" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -9358,10 +9354,10 @@
         <v>305</v>
       </c>
       <c r="D112" s="19" t="s">
+        <v>822</v>
+      </c>
+      <c r="E112" s="19" t="s">
         <v>823</v>
-      </c>
-      <c r="E112" s="19" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -9375,10 +9371,10 @@
         <v>305</v>
       </c>
       <c r="D113" s="20" t="s">
+        <v>822</v>
+      </c>
+      <c r="E113" s="20" t="s">
         <v>823</v>
-      </c>
-      <c r="E113" s="20" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -9392,10 +9388,10 @@
         <v>305</v>
       </c>
       <c r="D114" s="19" t="s">
+        <v>824</v>
+      </c>
+      <c r="E114" s="19" t="s">
         <v>825</v>
-      </c>
-      <c r="E114" s="19" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -9409,10 +9405,10 @@
         <v>305</v>
       </c>
       <c r="D115" s="20" t="s">
+        <v>672</v>
+      </c>
+      <c r="E115" s="20" t="s">
         <v>673</v>
-      </c>
-      <c r="E115" s="20" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -9426,10 +9422,10 @@
         <v>305</v>
       </c>
       <c r="D116" s="19" t="s">
+        <v>826</v>
+      </c>
+      <c r="E116" s="19" t="s">
         <v>827</v>
-      </c>
-      <c r="E116" s="19" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -9443,10 +9439,10 @@
         <v>305</v>
       </c>
       <c r="D117" s="20" t="s">
+        <v>828</v>
+      </c>
+      <c r="E117" s="20" t="s">
         <v>829</v>
-      </c>
-      <c r="E117" s="20" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -9460,10 +9456,10 @@
         <v>305</v>
       </c>
       <c r="D118" s="19" t="s">
+        <v>830</v>
+      </c>
+      <c r="E118" s="19" t="s">
         <v>831</v>
-      </c>
-      <c r="E118" s="19" t="s">
-        <v>832</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -9477,10 +9473,10 @@
         <v>305</v>
       </c>
       <c r="D119" s="20" t="s">
+        <v>832</v>
+      </c>
+      <c r="E119" s="20" t="s">
         <v>833</v>
-      </c>
-      <c r="E119" s="20" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -9494,10 +9490,10 @@
         <v>305</v>
       </c>
       <c r="D120" s="19" t="s">
+        <v>834</v>
+      </c>
+      <c r="E120" s="19" t="s">
         <v>835</v>
-      </c>
-      <c r="E120" s="19" t="s">
-        <v>836</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -9511,10 +9507,10 @@
         <v>305</v>
       </c>
       <c r="D121" s="20" t="s">
+        <v>836</v>
+      </c>
+      <c r="E121" s="20" t="s">
         <v>837</v>
-      </c>
-      <c r="E121" s="20" t="s">
-        <v>838</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -9528,10 +9524,10 @@
         <v>305</v>
       </c>
       <c r="D122" s="19" t="s">
+        <v>838</v>
+      </c>
+      <c r="E122" s="19" t="s">
         <v>839</v>
-      </c>
-      <c r="E122" s="19" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -9545,10 +9541,10 @@
         <v>305</v>
       </c>
       <c r="D123" s="20" t="s">
+        <v>840</v>
+      </c>
+      <c r="E123" s="20" t="s">
         <v>841</v>
-      </c>
-      <c r="E123" s="20" t="s">
-        <v>842</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -9562,10 +9558,10 @@
         <v>305</v>
       </c>
       <c r="D124" s="19" t="s">
+        <v>842</v>
+      </c>
+      <c r="E124" s="19" t="s">
         <v>843</v>
-      </c>
-      <c r="E124" s="19" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -9579,10 +9575,10 @@
         <v>305</v>
       </c>
       <c r="D125" s="20" t="s">
+        <v>844</v>
+      </c>
+      <c r="E125" s="20" t="s">
         <v>845</v>
-      </c>
-      <c r="E125" s="20" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -9596,10 +9592,10 @@
         <v>305</v>
       </c>
       <c r="D126" s="19" t="s">
+        <v>846</v>
+      </c>
+      <c r="E126" s="19" t="s">
         <v>847</v>
-      </c>
-      <c r="E126" s="19" t="s">
-        <v>848</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -9613,10 +9609,10 @@
         <v>305</v>
       </c>
       <c r="D127" s="20" t="s">
+        <v>848</v>
+      </c>
+      <c r="E127" s="20" t="s">
         <v>849</v>
-      </c>
-      <c r="E127" s="20" t="s">
-        <v>850</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -9630,10 +9626,10 @@
         <v>305</v>
       </c>
       <c r="D128" s="19" t="s">
+        <v>850</v>
+      </c>
+      <c r="E128" s="19" t="s">
         <v>851</v>
-      </c>
-      <c r="E128" s="19" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -9647,10 +9643,10 @@
         <v>305</v>
       </c>
       <c r="D129" s="20" t="s">
+        <v>852</v>
+      </c>
+      <c r="E129" s="20" t="s">
         <v>853</v>
-      </c>
-      <c r="E129" s="20" t="s">
-        <v>854</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -9664,10 +9660,10 @@
         <v>305</v>
       </c>
       <c r="D130" s="19" t="s">
+        <v>1107</v>
+      </c>
+      <c r="E130" s="19" t="s">
         <v>1108</v>
-      </c>
-      <c r="E130" s="19" t="s">
-        <v>1109</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -9681,10 +9677,10 @@
         <v>305</v>
       </c>
       <c r="D131" s="20" t="s">
+        <v>854</v>
+      </c>
+      <c r="E131" s="20" t="s">
         <v>855</v>
-      </c>
-      <c r="E131" s="20" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -9698,10 +9694,10 @@
         <v>305</v>
       </c>
       <c r="D132" s="19" t="s">
+        <v>856</v>
+      </c>
+      <c r="E132" s="19" t="s">
         <v>857</v>
-      </c>
-      <c r="E132" s="19" t="s">
-        <v>858</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -9715,10 +9711,10 @@
         <v>305</v>
       </c>
       <c r="D133" s="20" t="s">
+        <v>858</v>
+      </c>
+      <c r="E133" s="20" t="s">
         <v>859</v>
-      </c>
-      <c r="E133" s="20" t="s">
-        <v>860</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -9732,10 +9728,10 @@
         <v>305</v>
       </c>
       <c r="D134" s="19" t="s">
+        <v>860</v>
+      </c>
+      <c r="E134" s="19" t="s">
         <v>861</v>
-      </c>
-      <c r="E134" s="19" t="s">
-        <v>862</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -9749,10 +9745,10 @@
         <v>305</v>
       </c>
       <c r="D135" s="20" t="s">
+        <v>862</v>
+      </c>
+      <c r="E135" s="20" t="s">
         <v>863</v>
-      </c>
-      <c r="E135" s="20" t="s">
-        <v>864</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -9766,10 +9762,10 @@
         <v>305</v>
       </c>
       <c r="D136" s="19" t="s">
+        <v>864</v>
+      </c>
+      <c r="E136" s="19" t="s">
         <v>865</v>
-      </c>
-      <c r="E136" s="19" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -9783,10 +9779,10 @@
         <v>305</v>
       </c>
       <c r="D137" s="20" t="s">
+        <v>864</v>
+      </c>
+      <c r="E137" s="20" t="s">
         <v>865</v>
-      </c>
-      <c r="E137" s="20" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -9800,10 +9796,10 @@
         <v>305</v>
       </c>
       <c r="D138" s="19" t="s">
+        <v>866</v>
+      </c>
+      <c r="E138" s="19" t="s">
         <v>867</v>
-      </c>
-      <c r="E138" s="19" t="s">
-        <v>868</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -9817,10 +9813,10 @@
         <v>305</v>
       </c>
       <c r="D139" s="20" t="s">
+        <v>868</v>
+      </c>
+      <c r="E139" s="20" t="s">
         <v>869</v>
-      </c>
-      <c r="E139" s="20" t="s">
-        <v>870</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -9834,10 +9830,10 @@
         <v>305</v>
       </c>
       <c r="D140" s="19" t="s">
+        <v>870</v>
+      </c>
+      <c r="E140" s="19" t="s">
         <v>871</v>
-      </c>
-      <c r="E140" s="19" t="s">
-        <v>872</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -9851,10 +9847,10 @@
         <v>305</v>
       </c>
       <c r="D141" s="20" t="s">
+        <v>872</v>
+      </c>
+      <c r="E141" s="20" t="s">
         <v>873</v>
-      </c>
-      <c r="E141" s="20" t="s">
-        <v>874</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -9868,10 +9864,10 @@
         <v>305</v>
       </c>
       <c r="D142" s="19" t="s">
+        <v>874</v>
+      </c>
+      <c r="E142" s="19" t="s">
         <v>875</v>
-      </c>
-      <c r="E142" s="19" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -9885,10 +9881,10 @@
         <v>305</v>
       </c>
       <c r="D143" s="20" t="s">
+        <v>876</v>
+      </c>
+      <c r="E143" s="20" t="s">
         <v>877</v>
-      </c>
-      <c r="E143" s="20" t="s">
-        <v>878</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -9902,10 +9898,10 @@
         <v>305</v>
       </c>
       <c r="D144" s="19" t="s">
+        <v>878</v>
+      </c>
+      <c r="E144" s="19" t="s">
         <v>879</v>
-      </c>
-      <c r="E144" s="19" t="s">
-        <v>880</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -9919,10 +9915,10 @@
         <v>305</v>
       </c>
       <c r="D145" s="20" t="s">
+        <v>880</v>
+      </c>
+      <c r="E145" s="20" t="s">
         <v>881</v>
-      </c>
-      <c r="E145" s="20" t="s">
-        <v>882</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -9936,10 +9932,10 @@
         <v>305</v>
       </c>
       <c r="D146" s="19" t="s">
+        <v>882</v>
+      </c>
+      <c r="E146" s="19" t="s">
         <v>883</v>
-      </c>
-      <c r="E146" s="19" t="s">
-        <v>884</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -9953,10 +9949,10 @@
         <v>305</v>
       </c>
       <c r="D147" s="20" t="s">
+        <v>784</v>
+      </c>
+      <c r="E147" s="20" t="s">
         <v>785</v>
-      </c>
-      <c r="E147" s="20" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -9970,10 +9966,10 @@
         <v>305</v>
       </c>
       <c r="D148" s="19" t="s">
+        <v>884</v>
+      </c>
+      <c r="E148" s="19" t="s">
         <v>885</v>
-      </c>
-      <c r="E148" s="19" t="s">
-        <v>886</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -9987,10 +9983,10 @@
         <v>305</v>
       </c>
       <c r="D149" s="20" t="s">
+        <v>886</v>
+      </c>
+      <c r="E149" s="20" t="s">
         <v>887</v>
-      </c>
-      <c r="E149" s="20" t="s">
-        <v>888</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -10004,10 +10000,10 @@
         <v>305</v>
       </c>
       <c r="D150" s="19" t="s">
+        <v>888</v>
+      </c>
+      <c r="E150" s="19" t="s">
         <v>889</v>
-      </c>
-      <c r="E150" s="19" t="s">
-        <v>890</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -10021,10 +10017,10 @@
         <v>305</v>
       </c>
       <c r="D151" s="20" t="s">
+        <v>890</v>
+      </c>
+      <c r="E151" s="20" t="s">
         <v>891</v>
-      </c>
-      <c r="E151" s="20" t="s">
-        <v>892</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -10038,10 +10034,10 @@
         <v>305</v>
       </c>
       <c r="D152" s="19" t="s">
+        <v>892</v>
+      </c>
+      <c r="E152" s="19" t="s">
         <v>893</v>
-      </c>
-      <c r="E152" s="19" t="s">
-        <v>894</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -10055,10 +10051,10 @@
         <v>305</v>
       </c>
       <c r="D153" s="20" t="s">
+        <v>894</v>
+      </c>
+      <c r="E153" s="20" t="s">
         <v>895</v>
-      </c>
-      <c r="E153" s="20" t="s">
-        <v>896</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -10072,10 +10068,10 @@
         <v>305</v>
       </c>
       <c r="D154" s="19" t="s">
+        <v>896</v>
+      </c>
+      <c r="E154" s="19" t="s">
         <v>897</v>
-      </c>
-      <c r="E154" s="19" t="s">
-        <v>898</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -10089,10 +10085,10 @@
         <v>305</v>
       </c>
       <c r="D155" s="20" t="s">
+        <v>898</v>
+      </c>
+      <c r="E155" s="20" t="s">
         <v>899</v>
-      </c>
-      <c r="E155" s="20" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -10106,10 +10102,10 @@
         <v>305</v>
       </c>
       <c r="D156" s="19" t="s">
+        <v>900</v>
+      </c>
+      <c r="E156" s="19" t="s">
         <v>901</v>
-      </c>
-      <c r="E156" s="19" t="s">
-        <v>902</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -10123,10 +10119,10 @@
         <v>305</v>
       </c>
       <c r="D157" s="20" t="s">
+        <v>902</v>
+      </c>
+      <c r="E157" s="20" t="s">
         <v>903</v>
-      </c>
-      <c r="E157" s="20" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -10140,10 +10136,10 @@
         <v>305</v>
       </c>
       <c r="D158" s="19" t="s">
+        <v>904</v>
+      </c>
+      <c r="E158" s="19" t="s">
         <v>905</v>
-      </c>
-      <c r="E158" s="19" t="s">
-        <v>906</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -10157,10 +10153,10 @@
         <v>305</v>
       </c>
       <c r="D159" s="20" t="s">
+        <v>906</v>
+      </c>
+      <c r="E159" s="20" t="s">
         <v>907</v>
-      </c>
-      <c r="E159" s="20" t="s">
-        <v>908</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -10174,10 +10170,10 @@
         <v>305</v>
       </c>
       <c r="D160" s="19" t="s">
+        <v>908</v>
+      </c>
+      <c r="E160" s="19" t="s">
         <v>909</v>
-      </c>
-      <c r="E160" s="19" t="s">
-        <v>910</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -10191,10 +10187,10 @@
         <v>305</v>
       </c>
       <c r="D161" s="20" t="s">
+        <v>910</v>
+      </c>
+      <c r="E161" s="20" t="s">
         <v>911</v>
-      </c>
-      <c r="E161" s="20" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -10208,10 +10204,10 @@
         <v>305</v>
       </c>
       <c r="D162" s="19" t="s">
+        <v>912</v>
+      </c>
+      <c r="E162" s="19" t="s">
         <v>913</v>
-      </c>
-      <c r="E162" s="19" t="s">
-        <v>914</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -10225,10 +10221,10 @@
         <v>305</v>
       </c>
       <c r="D163" s="20" t="s">
+        <v>914</v>
+      </c>
+      <c r="E163" s="20" t="s">
         <v>915</v>
-      </c>
-      <c r="E163" s="20" t="s">
-        <v>916</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -10242,10 +10238,10 @@
         <v>305</v>
       </c>
       <c r="D164" s="19" t="s">
+        <v>916</v>
+      </c>
+      <c r="E164" s="19" t="s">
         <v>917</v>
-      </c>
-      <c r="E164" s="19" t="s">
-        <v>918</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -10259,10 +10255,10 @@
         <v>305</v>
       </c>
       <c r="D165" s="20" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E165" s="20" t="s">
         <v>1116</v>
-      </c>
-      <c r="E165" s="20" t="s">
-        <v>1117</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -10276,10 +10272,10 @@
         <v>305</v>
       </c>
       <c r="D166" s="19" t="s">
+        <v>918</v>
+      </c>
+      <c r="E166" s="19" t="s">
         <v>919</v>
-      </c>
-      <c r="E166" s="19" t="s">
-        <v>920</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -10293,10 +10289,10 @@
         <v>305</v>
       </c>
       <c r="D167" s="20" t="s">
+        <v>920</v>
+      </c>
+      <c r="E167" s="20" t="s">
         <v>921</v>
-      </c>
-      <c r="E167" s="20" t="s">
-        <v>922</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -10310,10 +10306,10 @@
         <v>305</v>
       </c>
       <c r="D168" s="19" t="s">
+        <v>922</v>
+      </c>
+      <c r="E168" s="19" t="s">
         <v>923</v>
-      </c>
-      <c r="E168" s="19" t="s">
-        <v>924</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -10327,10 +10323,10 @@
         <v>305</v>
       </c>
       <c r="D169" s="20" t="s">
+        <v>924</v>
+      </c>
+      <c r="E169" s="20" t="s">
         <v>925</v>
-      </c>
-      <c r="E169" s="20" t="s">
-        <v>926</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -10344,10 +10340,10 @@
         <v>305</v>
       </c>
       <c r="D170" s="19" t="s">
+        <v>926</v>
+      </c>
+      <c r="E170" s="19" t="s">
         <v>927</v>
-      </c>
-      <c r="E170" s="19" t="s">
-        <v>928</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -10361,10 +10357,10 @@
         <v>305</v>
       </c>
       <c r="D171" s="20" t="s">
+        <v>928</v>
+      </c>
+      <c r="E171" s="20" t="s">
         <v>929</v>
-      </c>
-      <c r="E171" s="20" t="s">
-        <v>930</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -10378,10 +10374,10 @@
         <v>305</v>
       </c>
       <c r="D172" s="19" t="s">
+        <v>930</v>
+      </c>
+      <c r="E172" s="19" t="s">
         <v>931</v>
-      </c>
-      <c r="E172" s="19" t="s">
-        <v>932</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -10395,10 +10391,10 @@
         <v>305</v>
       </c>
       <c r="D173" s="20" t="s">
+        <v>932</v>
+      </c>
+      <c r="E173" s="20" t="s">
         <v>933</v>
-      </c>
-      <c r="E173" s="20" t="s">
-        <v>934</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -10412,10 +10408,10 @@
         <v>305</v>
       </c>
       <c r="D174" s="19" t="s">
+        <v>934</v>
+      </c>
+      <c r="E174" s="19" t="s">
         <v>935</v>
-      </c>
-      <c r="E174" s="19" t="s">
-        <v>936</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -10429,10 +10425,10 @@
         <v>305</v>
       </c>
       <c r="D175" s="20" t="s">
+        <v>936</v>
+      </c>
+      <c r="E175" s="20" t="s">
         <v>937</v>
-      </c>
-      <c r="E175" s="20" t="s">
-        <v>938</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -10446,10 +10442,10 @@
         <v>305</v>
       </c>
       <c r="D176" s="19" t="s">
+        <v>938</v>
+      </c>
+      <c r="E176" s="19" t="s">
         <v>939</v>
-      </c>
-      <c r="E176" s="19" t="s">
-        <v>940</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -10463,10 +10459,10 @@
         <v>305</v>
       </c>
       <c r="D177" s="20" t="s">
+        <v>938</v>
+      </c>
+      <c r="E177" s="20" t="s">
         <v>939</v>
-      </c>
-      <c r="E177" s="20" t="s">
-        <v>940</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -10480,10 +10476,10 @@
         <v>305</v>
       </c>
       <c r="D178" s="19" t="s">
+        <v>940</v>
+      </c>
+      <c r="E178" s="19" t="s">
         <v>941</v>
-      </c>
-      <c r="E178" s="19" t="s">
-        <v>942</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -10497,10 +10493,10 @@
         <v>305</v>
       </c>
       <c r="D179" s="20" t="s">
+        <v>924</v>
+      </c>
+      <c r="E179" s="20" t="s">
         <v>925</v>
-      </c>
-      <c r="E179" s="20" t="s">
-        <v>926</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -10514,10 +10510,10 @@
         <v>305</v>
       </c>
       <c r="D180" s="19" t="s">
+        <v>938</v>
+      </c>
+      <c r="E180" s="19" t="s">
         <v>939</v>
-      </c>
-      <c r="E180" s="19" t="s">
-        <v>940</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -10531,10 +10527,10 @@
         <v>305</v>
       </c>
       <c r="D181" s="20" t="s">
+        <v>942</v>
+      </c>
+      <c r="E181" s="20" t="s">
         <v>943</v>
-      </c>
-      <c r="E181" s="20" t="s">
-        <v>944</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -10548,10 +10544,10 @@
         <v>305</v>
       </c>
       <c r="D182" s="19" t="s">
+        <v>944</v>
+      </c>
+      <c r="E182" s="19" t="s">
         <v>945</v>
-      </c>
-      <c r="E182" s="19" t="s">
-        <v>946</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -10565,10 +10561,10 @@
         <v>305</v>
       </c>
       <c r="D183" s="20" t="s">
+        <v>946</v>
+      </c>
+      <c r="E183" s="20" t="s">
         <v>947</v>
-      </c>
-      <c r="E183" s="20" t="s">
-        <v>948</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -10582,10 +10578,10 @@
         <v>305</v>
       </c>
       <c r="D184" s="19" t="s">
+        <v>948</v>
+      </c>
+      <c r="E184" s="19" t="s">
         <v>949</v>
-      </c>
-      <c r="E184" s="19" t="s">
-        <v>950</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -10599,10 +10595,10 @@
         <v>305</v>
       </c>
       <c r="D185" s="20" t="s">
+        <v>950</v>
+      </c>
+      <c r="E185" s="20" t="s">
         <v>951</v>
-      </c>
-      <c r="E185" s="20" t="s">
-        <v>952</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -10616,10 +10612,10 @@
         <v>305</v>
       </c>
       <c r="D186" s="19" t="s">
+        <v>952</v>
+      </c>
+      <c r="E186" s="19" t="s">
         <v>953</v>
-      </c>
-      <c r="E186" s="19" t="s">
-        <v>954</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -10633,10 +10629,10 @@
         <v>305</v>
       </c>
       <c r="D187" s="20" t="s">
+        <v>950</v>
+      </c>
+      <c r="E187" s="20" t="s">
         <v>951</v>
-      </c>
-      <c r="E187" s="20" t="s">
-        <v>952</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -10650,10 +10646,10 @@
         <v>305</v>
       </c>
       <c r="D188" s="19" t="s">
+        <v>954</v>
+      </c>
+      <c r="E188" s="19" t="s">
         <v>955</v>
-      </c>
-      <c r="E188" s="19" t="s">
-        <v>956</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -10667,10 +10663,10 @@
         <v>305</v>
       </c>
       <c r="D189" s="20" t="s">
+        <v>950</v>
+      </c>
+      <c r="E189" s="20" t="s">
         <v>951</v>
-      </c>
-      <c r="E189" s="20" t="s">
-        <v>952</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -10684,10 +10680,10 @@
         <v>305</v>
       </c>
       <c r="D190" s="19" t="s">
+        <v>956</v>
+      </c>
+      <c r="E190" s="19" t="s">
         <v>957</v>
-      </c>
-      <c r="E190" s="19" t="s">
-        <v>958</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -10701,10 +10697,10 @@
         <v>305</v>
       </c>
       <c r="D191" s="20" t="s">
+        <v>672</v>
+      </c>
+      <c r="E191" s="20" t="s">
         <v>673</v>
-      </c>
-      <c r="E191" s="20" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -10718,10 +10714,10 @@
         <v>305</v>
       </c>
       <c r="D192" s="19" t="s">
+        <v>958</v>
+      </c>
+      <c r="E192" s="19" t="s">
         <v>959</v>
-      </c>
-      <c r="E192" s="19" t="s">
-        <v>960</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -10735,10 +10731,10 @@
         <v>305</v>
       </c>
       <c r="D193" s="20" t="s">
+        <v>960</v>
+      </c>
+      <c r="E193" s="20" t="s">
         <v>961</v>
-      </c>
-      <c r="E193" s="20" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -10752,10 +10748,10 @@
         <v>305</v>
       </c>
       <c r="D194" s="19" t="s">
+        <v>962</v>
+      </c>
+      <c r="E194" s="19" t="s">
         <v>963</v>
-      </c>
-      <c r="E194" s="19" t="s">
-        <v>964</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -10769,10 +10765,10 @@
         <v>305</v>
       </c>
       <c r="D195" s="20" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="E195" s="20" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -10786,10 +10782,10 @@
         <v>305</v>
       </c>
       <c r="D196" s="19" t="s">
+        <v>965</v>
+      </c>
+      <c r="E196" s="19" t="s">
         <v>966</v>
-      </c>
-      <c r="E196" s="19" t="s">
-        <v>967</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -10803,10 +10799,10 @@
         <v>305</v>
       </c>
       <c r="D197" s="20" t="s">
+        <v>967</v>
+      </c>
+      <c r="E197" s="20" t="s">
         <v>968</v>
-      </c>
-      <c r="E197" s="20" t="s">
-        <v>969</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -10820,10 +10816,10 @@
         <v>305</v>
       </c>
       <c r="D198" s="19" t="s">
+        <v>969</v>
+      </c>
+      <c r="E198" s="19" t="s">
         <v>970</v>
-      </c>
-      <c r="E198" s="19" t="s">
-        <v>971</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -10837,10 +10833,10 @@
         <v>305</v>
       </c>
       <c r="D199" s="20" t="s">
+        <v>971</v>
+      </c>
+      <c r="E199" s="20" t="s">
         <v>972</v>
-      </c>
-      <c r="E199" s="20" t="s">
-        <v>973</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -10854,10 +10850,10 @@
         <v>305</v>
       </c>
       <c r="D200" s="19" t="s">
+        <v>973</v>
+      </c>
+      <c r="E200" s="19" t="s">
         <v>974</v>
-      </c>
-      <c r="E200" s="19" t="s">
-        <v>975</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -10871,10 +10867,10 @@
         <v>305</v>
       </c>
       <c r="D201" s="20" t="s">
+        <v>975</v>
+      </c>
+      <c r="E201" s="20" t="s">
         <v>976</v>
-      </c>
-      <c r="E201" s="20" t="s">
-        <v>977</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -10888,10 +10884,10 @@
         <v>305</v>
       </c>
       <c r="D202" s="19" t="s">
+        <v>977</v>
+      </c>
+      <c r="E202" s="19" t="s">
         <v>978</v>
-      </c>
-      <c r="E202" s="19" t="s">
-        <v>979</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -10905,10 +10901,10 @@
         <v>305</v>
       </c>
       <c r="D203" s="20" t="s">
+        <v>979</v>
+      </c>
+      <c r="E203" s="20" t="s">
         <v>980</v>
-      </c>
-      <c r="E203" s="20" t="s">
-        <v>981</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -10922,10 +10918,10 @@
         <v>305</v>
       </c>
       <c r="D204" s="19" t="s">
+        <v>981</v>
+      </c>
+      <c r="E204" s="19" t="s">
         <v>982</v>
-      </c>
-      <c r="E204" s="19" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -10939,15 +10935,15 @@
         <v>305</v>
       </c>
       <c r="D205" s="20" t="s">
+        <v>983</v>
+      </c>
+      <c r="E205" s="20" t="s">
         <v>984</v>
-      </c>
-      <c r="E205" s="20" t="s">
-        <v>985</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="18" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B206" s="18" t="s">
         <v>304</v>
@@ -10956,10 +10952,10 @@
         <v>305</v>
       </c>
       <c r="D206" s="19" t="s">
+        <v>1118</v>
+      </c>
+      <c r="E206" s="19" t="s">
         <v>1119</v>
-      </c>
-      <c r="E206" s="19" t="s">
-        <v>1120</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -10973,10 +10969,10 @@
         <v>305</v>
       </c>
       <c r="D207" s="20" t="s">
+        <v>985</v>
+      </c>
+      <c r="E207" s="20" t="s">
         <v>986</v>
-      </c>
-      <c r="E207" s="20" t="s">
-        <v>987</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -10990,10 +10986,10 @@
         <v>305</v>
       </c>
       <c r="D208" s="19" t="s">
+        <v>987</v>
+      </c>
+      <c r="E208" s="19" t="s">
         <v>988</v>
-      </c>
-      <c r="E208" s="19" t="s">
-        <v>989</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -11007,10 +11003,10 @@
         <v>305</v>
       </c>
       <c r="D209" s="20" t="s">
+        <v>989</v>
+      </c>
+      <c r="E209" s="20" t="s">
         <v>990</v>
-      </c>
-      <c r="E209" s="20" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -11024,10 +11020,10 @@
         <v>305</v>
       </c>
       <c r="D210" s="19" t="s">
+        <v>991</v>
+      </c>
+      <c r="E210" s="19" t="s">
         <v>992</v>
-      </c>
-      <c r="E210" s="19" t="s">
-        <v>993</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -11041,10 +11037,10 @@
         <v>305</v>
       </c>
       <c r="D211" s="20" t="s">
+        <v>987</v>
+      </c>
+      <c r="E211" s="20" t="s">
         <v>988</v>
-      </c>
-      <c r="E211" s="20" t="s">
-        <v>989</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -11058,10 +11054,10 @@
         <v>305</v>
       </c>
       <c r="D212" s="19" t="s">
+        <v>993</v>
+      </c>
+      <c r="E212" s="19" t="s">
         <v>994</v>
-      </c>
-      <c r="E212" s="19" t="s">
-        <v>995</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -11075,10 +11071,10 @@
         <v>305</v>
       </c>
       <c r="D213" s="20" t="s">
+        <v>995</v>
+      </c>
+      <c r="E213" s="20" t="s">
         <v>996</v>
-      </c>
-      <c r="E213" s="20" t="s">
-        <v>997</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -11092,10 +11088,10 @@
         <v>305</v>
       </c>
       <c r="D214" s="19" t="s">
+        <v>997</v>
+      </c>
+      <c r="E214" s="19" t="s">
         <v>998</v>
-      </c>
-      <c r="E214" s="19" t="s">
-        <v>999</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -11109,10 +11105,10 @@
         <v>305</v>
       </c>
       <c r="D215" s="20" t="s">
+        <v>999</v>
+      </c>
+      <c r="E215" s="20" t="s">
         <v>1000</v>
-      </c>
-      <c r="E215" s="20" t="s">
-        <v>1001</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -11126,10 +11122,10 @@
         <v>305</v>
       </c>
       <c r="D216" s="19" t="s">
+        <v>1001</v>
+      </c>
+      <c r="E216" s="19" t="s">
         <v>1002</v>
-      </c>
-      <c r="E216" s="19" t="s">
-        <v>1003</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -11143,10 +11139,10 @@
         <v>305</v>
       </c>
       <c r="D217" s="20" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E217" s="20" t="s">
         <v>1004</v>
-      </c>
-      <c r="E217" s="20" t="s">
-        <v>1005</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
@@ -11160,10 +11156,10 @@
         <v>305</v>
       </c>
       <c r="D218" s="19" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E218" s="19" t="s">
         <v>1006</v>
-      </c>
-      <c r="E218" s="19" t="s">
-        <v>1007</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -11177,10 +11173,10 @@
         <v>305</v>
       </c>
       <c r="D219" s="20" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E219" s="20" t="s">
         <v>1004</v>
-      </c>
-      <c r="E219" s="20" t="s">
-        <v>1005</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -11194,10 +11190,10 @@
         <v>305</v>
       </c>
       <c r="D220" s="19" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E220" s="19" t="s">
         <v>1008</v>
-      </c>
-      <c r="E220" s="19" t="s">
-        <v>1009</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
@@ -11211,10 +11207,10 @@
         <v>305</v>
       </c>
       <c r="D221" s="20" t="s">
+        <v>1009</v>
+      </c>
+      <c r="E221" s="20" t="s">
         <v>1010</v>
-      </c>
-      <c r="E221" s="20" t="s">
-        <v>1011</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
@@ -11228,10 +11224,10 @@
         <v>305</v>
       </c>
       <c r="D222" s="19" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E222" s="19" t="s">
         <v>1012</v>
-      </c>
-      <c r="E222" s="19" t="s">
-        <v>1013</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -11245,10 +11241,10 @@
         <v>305</v>
       </c>
       <c r="D223" s="20" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E223" s="20" t="s">
         <v>1014</v>
-      </c>
-      <c r="E223" s="20" t="s">
-        <v>1015</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -11262,10 +11258,10 @@
         <v>305</v>
       </c>
       <c r="D224" s="19" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E224" s="19" t="s">
         <v>1014</v>
-      </c>
-      <c r="E224" s="19" t="s">
-        <v>1015</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -11279,10 +11275,10 @@
         <v>305</v>
       </c>
       <c r="D225" s="20" t="s">
+        <v>672</v>
+      </c>
+      <c r="E225" s="20" t="s">
         <v>673</v>
-      </c>
-      <c r="E225" s="20" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
@@ -11296,10 +11292,10 @@
         <v>305</v>
       </c>
       <c r="D226" s="19" t="s">
+        <v>672</v>
+      </c>
+      <c r="E226" s="19" t="s">
         <v>673</v>
-      </c>
-      <c r="E226" s="19" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
@@ -11313,10 +11309,10 @@
         <v>305</v>
       </c>
       <c r="D227" s="20" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E227" s="20" t="s">
         <v>1016</v>
-      </c>
-      <c r="E227" s="20" t="s">
-        <v>1017</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
@@ -11330,10 +11326,10 @@
         <v>305</v>
       </c>
       <c r="D228" s="19" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E228" s="19" t="s">
         <v>1018</v>
-      </c>
-      <c r="E228" s="19" t="s">
-        <v>1019</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -11347,10 +11343,10 @@
         <v>305</v>
       </c>
       <c r="D229" s="20" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E229" s="20" t="s">
         <v>1020</v>
-      </c>
-      <c r="E229" s="20" t="s">
-        <v>1021</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
@@ -11364,10 +11360,10 @@
         <v>305</v>
       </c>
       <c r="D230" s="19" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E230" s="19" t="s">
         <v>1022</v>
-      </c>
-      <c r="E230" s="19" t="s">
-        <v>1023</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -11381,10 +11377,10 @@
         <v>305</v>
       </c>
       <c r="D231" s="20" t="s">
+        <v>1023</v>
+      </c>
+      <c r="E231" s="20" t="s">
         <v>1024</v>
-      </c>
-      <c r="E231" s="20" t="s">
-        <v>1025</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
@@ -11398,10 +11394,10 @@
         <v>305</v>
       </c>
       <c r="D232" s="19" t="s">
+        <v>672</v>
+      </c>
+      <c r="E232" s="19" t="s">
         <v>673</v>
-      </c>
-      <c r="E232" s="19" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
@@ -11415,10 +11411,10 @@
         <v>305</v>
       </c>
       <c r="D233" s="20" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E233" s="20" t="s">
         <v>1026</v>
-      </c>
-      <c r="E233" s="20" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
@@ -11432,10 +11428,10 @@
         <v>305</v>
       </c>
       <c r="D234" s="19" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E234" s="19" t="s">
         <v>1028</v>
-      </c>
-      <c r="E234" s="19" t="s">
-        <v>1029</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
@@ -11449,10 +11445,10 @@
         <v>305</v>
       </c>
       <c r="D235" s="20" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E235" s="20" t="s">
         <v>1030</v>
-      </c>
-      <c r="E235" s="20" t="s">
-        <v>1031</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
@@ -11466,10 +11462,10 @@
         <v>305</v>
       </c>
       <c r="D236" s="19" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E236" s="19" t="s">
         <v>1032</v>
-      </c>
-      <c r="E236" s="19" t="s">
-        <v>1033</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
@@ -11483,10 +11479,10 @@
         <v>305</v>
       </c>
       <c r="D237" s="20" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E237" s="20" t="s">
         <v>1034</v>
-      </c>
-      <c r="E237" s="20" t="s">
-        <v>1035</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
@@ -11500,10 +11496,10 @@
         <v>305</v>
       </c>
       <c r="D238" s="19" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E238" s="19" t="s">
         <v>1036</v>
-      </c>
-      <c r="E238" s="19" t="s">
-        <v>1037</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
@@ -11517,10 +11513,10 @@
         <v>305</v>
       </c>
       <c r="D239" s="20" t="s">
+        <v>1037</v>
+      </c>
+      <c r="E239" s="20" t="s">
         <v>1038</v>
-      </c>
-      <c r="E239" s="20" t="s">
-        <v>1039</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
@@ -11534,10 +11530,10 @@
         <v>305</v>
       </c>
       <c r="D240" s="19" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E240" s="19" t="s">
         <v>1040</v>
-      </c>
-      <c r="E240" s="19" t="s">
-        <v>1041</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -11551,10 +11547,10 @@
         <v>305</v>
       </c>
       <c r="D241" s="20" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E241" s="20" t="s">
         <v>1042</v>
-      </c>
-      <c r="E241" s="20" t="s">
-        <v>1043</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
@@ -11568,10 +11564,10 @@
         <v>305</v>
       </c>
       <c r="D242" s="19" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E242" s="19" t="s">
         <v>1044</v>
-      </c>
-      <c r="E242" s="19" t="s">
-        <v>1045</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
@@ -11585,10 +11581,10 @@
         <v>305</v>
       </c>
       <c r="D243" s="20" t="s">
+        <v>1045</v>
+      </c>
+      <c r="E243" s="20" t="s">
         <v>1046</v>
-      </c>
-      <c r="E243" s="20" t="s">
-        <v>1047</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
@@ -11602,10 +11598,10 @@
         <v>305</v>
       </c>
       <c r="D244" s="19" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E244" s="19" t="s">
         <v>1048</v>
-      </c>
-      <c r="E244" s="19" t="s">
-        <v>1049</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -11619,10 +11615,10 @@
         <v>305</v>
       </c>
       <c r="D245" s="20" t="s">
+        <v>1049</v>
+      </c>
+      <c r="E245" s="20" t="s">
         <v>1050</v>
-      </c>
-      <c r="E245" s="20" t="s">
-        <v>1051</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -11636,10 +11632,10 @@
         <v>305</v>
       </c>
       <c r="D246" s="19" t="s">
+        <v>672</v>
+      </c>
+      <c r="E246" s="19" t="s">
         <v>673</v>
-      </c>
-      <c r="E246" s="19" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -11653,10 +11649,10 @@
         <v>305</v>
       </c>
       <c r="D247" s="20" t="s">
+        <v>672</v>
+      </c>
+      <c r="E247" s="20" t="s">
         <v>673</v>
-      </c>
-      <c r="E247" s="20" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
@@ -11670,10 +11666,10 @@
         <v>305</v>
       </c>
       <c r="D248" s="19" t="s">
+        <v>672</v>
+      </c>
+      <c r="E248" s="19" t="s">
         <v>673</v>
-      </c>
-      <c r="E248" s="19" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
@@ -11687,10 +11683,10 @@
         <v>305</v>
       </c>
       <c r="D249" s="20" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E249" s="20" t="s">
         <v>1052</v>
-      </c>
-      <c r="E249" s="20" t="s">
-        <v>1053</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
@@ -11704,10 +11700,10 @@
         <v>305</v>
       </c>
       <c r="D250" s="19" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E250" s="19" t="s">
         <v>1054</v>
-      </c>
-      <c r="E250" s="19" t="s">
-        <v>1055</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
@@ -11721,10 +11717,10 @@
         <v>305</v>
       </c>
       <c r="D251" s="20" t="s">
+        <v>1055</v>
+      </c>
+      <c r="E251" s="20" t="s">
         <v>1056</v>
-      </c>
-      <c r="E251" s="20" t="s">
-        <v>1057</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
@@ -11738,10 +11734,10 @@
         <v>305</v>
       </c>
       <c r="D252" s="19" t="s">
+        <v>1057</v>
+      </c>
+      <c r="E252" s="19" t="s">
         <v>1058</v>
-      </c>
-      <c r="E252" s="19" t="s">
-        <v>1059</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
@@ -11755,10 +11751,10 @@
         <v>305</v>
       </c>
       <c r="D253" s="20" t="s">
+        <v>1111</v>
+      </c>
+      <c r="E253" s="20" t="s">
         <v>1112</v>
-      </c>
-      <c r="E253" s="20" t="s">
-        <v>1113</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -11772,10 +11768,10 @@
         <v>305</v>
       </c>
       <c r="D254" s="19" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E254" s="19" t="s">
         <v>1060</v>
-      </c>
-      <c r="E254" s="19" t="s">
-        <v>1061</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
@@ -11789,10 +11785,10 @@
         <v>305</v>
       </c>
       <c r="D255" s="20" t="s">
+        <v>1061</v>
+      </c>
+      <c r="E255" s="20" t="s">
         <v>1062</v>
-      </c>
-      <c r="E255" s="20" t="s">
-        <v>1063</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
@@ -11806,10 +11802,10 @@
         <v>305</v>
       </c>
       <c r="D256" s="19" t="s">
+        <v>672</v>
+      </c>
+      <c r="E256" s="19" t="s">
         <v>673</v>
-      </c>
-      <c r="E256" s="19" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
@@ -11823,10 +11819,10 @@
         <v>305</v>
       </c>
       <c r="D257" s="20" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E257" s="20" t="s">
         <v>1064</v>
-      </c>
-      <c r="E257" s="20" t="s">
-        <v>1065</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -11840,10 +11836,10 @@
         <v>305</v>
       </c>
       <c r="D258" s="19" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E258" s="19" t="s">
         <v>1042</v>
-      </c>
-      <c r="E258" s="19" t="s">
-        <v>1043</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
@@ -11857,10 +11853,10 @@
         <v>305</v>
       </c>
       <c r="D259" s="20" t="s">
+        <v>672</v>
+      </c>
+      <c r="E259" s="20" t="s">
         <v>673</v>
-      </c>
-      <c r="E259" s="20" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -11874,10 +11870,10 @@
         <v>305</v>
       </c>
       <c r="D260" s="19" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E260" s="19" t="s">
         <v>1066</v>
-      </c>
-      <c r="E260" s="19" t="s">
-        <v>1067</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -11891,10 +11887,10 @@
         <v>305</v>
       </c>
       <c r="D261" s="20" t="s">
+        <v>672</v>
+      </c>
+      <c r="E261" s="20" t="s">
         <v>673</v>
-      </c>
-      <c r="E261" s="20" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
@@ -11908,10 +11904,10 @@
         <v>305</v>
       </c>
       <c r="D262" s="19" t="s">
+        <v>672</v>
+      </c>
+      <c r="E262" s="19" t="s">
         <v>673</v>
-      </c>
-      <c r="E262" s="19" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
@@ -11925,10 +11921,10 @@
         <v>305</v>
       </c>
       <c r="D263" s="20" t="s">
+        <v>1067</v>
+      </c>
+      <c r="E263" s="20" t="s">
         <v>1068</v>
-      </c>
-      <c r="E263" s="20" t="s">
-        <v>1069</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
@@ -11942,10 +11938,10 @@
         <v>305</v>
       </c>
       <c r="D264" s="19" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E264" s="19" t="s">
         <v>1070</v>
-      </c>
-      <c r="E264" s="19" t="s">
-        <v>1071</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
@@ -11959,10 +11955,10 @@
         <v>305</v>
       </c>
       <c r="D265" s="20" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E265" s="20" t="s">
         <v>1072</v>
-      </c>
-      <c r="E265" s="20" t="s">
-        <v>1073</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
@@ -11976,10 +11972,10 @@
         <v>305</v>
       </c>
       <c r="D266" s="19" t="s">
+        <v>672</v>
+      </c>
+      <c r="E266" s="19" t="s">
         <v>673</v>
-      </c>
-      <c r="E266" s="19" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
@@ -11993,10 +11989,10 @@
         <v>305</v>
       </c>
       <c r="D267" s="20" t="s">
+        <v>672</v>
+      </c>
+      <c r="E267" s="20" t="s">
         <v>673</v>
-      </c>
-      <c r="E267" s="20" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
@@ -12010,10 +12006,10 @@
         <v>305</v>
       </c>
       <c r="D268" s="19" t="s">
+        <v>1073</v>
+      </c>
+      <c r="E268" s="19" t="s">
         <v>1074</v>
-      </c>
-      <c r="E268" s="19" t="s">
-        <v>1075</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
@@ -12027,15 +12023,15 @@
         <v>305</v>
       </c>
       <c r="D269" s="20" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E269" s="20" t="s">
         <v>1076</v>
-      </c>
-      <c r="E269" s="20" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="18" t="s">
-        <v>608</v>
+        <v>1121</v>
       </c>
       <c r="B270" s="18" t="s">
         <v>304</v>
@@ -12044,15 +12040,15 @@
         <v>305</v>
       </c>
       <c r="D270" s="19" t="s">
+        <v>672</v>
+      </c>
+      <c r="E270" s="19" t="s">
         <v>673</v>
-      </c>
-      <c r="E270" s="19" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="18" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B271" s="18" t="s">
         <v>304</v>
@@ -12061,15 +12057,15 @@
         <v>305</v>
       </c>
       <c r="D271" s="20" t="s">
+        <v>1077</v>
+      </c>
+      <c r="E271" s="20" t="s">
         <v>1078</v>
-      </c>
-      <c r="E271" s="20" t="s">
-        <v>1079</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="18" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B272" s="18" t="s">
         <v>304</v>
@@ -12078,15 +12074,15 @@
         <v>305</v>
       </c>
       <c r="D272" s="19" t="s">
+        <v>672</v>
+      </c>
+      <c r="E272" s="19" t="s">
         <v>673</v>
-      </c>
-      <c r="E272" s="19" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="18" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B273" s="18" t="s">
         <v>304</v>
@@ -12095,15 +12091,15 @@
         <v>305</v>
       </c>
       <c r="D273" s="20" t="s">
+        <v>1079</v>
+      </c>
+      <c r="E273" s="20" t="s">
         <v>1080</v>
-      </c>
-      <c r="E273" s="20" t="s">
-        <v>1081</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="18" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B274" s="18" t="s">
         <v>304</v>
@@ -12112,15 +12108,15 @@
         <v>305</v>
       </c>
       <c r="D274" s="19" t="s">
+        <v>1081</v>
+      </c>
+      <c r="E274" s="19" t="s">
         <v>1082</v>
-      </c>
-      <c r="E274" s="19" t="s">
-        <v>1083</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="18" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B275" s="18" t="s">
         <v>304</v>
@@ -12129,15 +12125,15 @@
         <v>305</v>
       </c>
       <c r="D275" s="20" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E275" s="20" t="s">
         <v>1084</v>
-      </c>
-      <c r="E275" s="20" t="s">
-        <v>1085</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="18" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B276" s="18" t="s">
         <v>304</v>
@@ -12146,15 +12142,15 @@
         <v>305</v>
       </c>
       <c r="D276" s="19" t="s">
+        <v>1085</v>
+      </c>
+      <c r="E276" s="19" t="s">
         <v>1086</v>
-      </c>
-      <c r="E276" s="19" t="s">
-        <v>1087</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="18" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B277" s="18" t="s">
         <v>304</v>
@@ -12163,15 +12159,15 @@
         <v>305</v>
       </c>
       <c r="D277" s="20" t="s">
+        <v>1087</v>
+      </c>
+      <c r="E277" s="20" t="s">
         <v>1088</v>
-      </c>
-      <c r="E277" s="20" t="s">
-        <v>1089</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="18" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B278" s="18" t="s">
         <v>304</v>
@@ -12180,15 +12176,15 @@
         <v>305</v>
       </c>
       <c r="D278" s="19" t="s">
+        <v>672</v>
+      </c>
+      <c r="E278" s="19" t="s">
         <v>673</v>
-      </c>
-      <c r="E278" s="19" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="18" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B279" s="18" t="s">
         <v>304</v>
@@ -12197,15 +12193,15 @@
         <v>305</v>
       </c>
       <c r="D279" s="20" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E279" s="20" t="s">
         <v>1090</v>
-      </c>
-      <c r="E279" s="20" t="s">
-        <v>1091</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="18" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B280" s="18" t="s">
         <v>304</v>
@@ -12214,15 +12210,15 @@
         <v>305</v>
       </c>
       <c r="D280" s="19" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E280" s="19" t="s">
         <v>1092</v>
-      </c>
-      <c r="E280" s="19" t="s">
-        <v>1093</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="18" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B281" s="18" t="s">
         <v>304</v>
@@ -12231,15 +12227,15 @@
         <v>305</v>
       </c>
       <c r="D281" s="20" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E281" s="20" t="s">
         <v>1094</v>
-      </c>
-      <c r="E281" s="20" t="s">
-        <v>1095</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="18" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B282" s="18" t="s">
         <v>304</v>
@@ -12248,15 +12244,15 @@
         <v>305</v>
       </c>
       <c r="D282" s="19" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E282" s="19" t="s">
         <v>1096</v>
-      </c>
-      <c r="E282" s="19" t="s">
-        <v>1097</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="18" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B283" s="18" t="s">
         <v>304</v>
@@ -12265,15 +12261,15 @@
         <v>305</v>
       </c>
       <c r="D283" s="20" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E283" s="20" t="s">
         <v>1098</v>
-      </c>
-      <c r="E283" s="20" t="s">
-        <v>1099</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="18" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B284" s="18" t="s">
         <v>343</v>
@@ -12282,66 +12278,66 @@
         <v>305</v>
       </c>
       <c r="D284" s="19" t="s">
+        <v>1099</v>
+      </c>
+      <c r="E284" s="19" t="s">
         <v>1100</v>
-      </c>
-      <c r="E284" s="19" t="s">
-        <v>1101</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="18" t="s">
+        <v>622</v>
+      </c>
+      <c r="B285" s="18" t="s">
         <v>623</v>
       </c>
-      <c r="B285" s="18" t="s">
-        <v>624</v>
-      </c>
       <c r="C285" s="18" t="s">
         <v>305</v>
       </c>
       <c r="D285" s="20" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E285" s="20" t="s">
         <v>1102</v>
-      </c>
-      <c r="E285" s="20" t="s">
-        <v>1103</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="18" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B286" s="18" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C286" s="18" t="s">
         <v>305</v>
       </c>
       <c r="D286" s="19" t="s">
+        <v>1103</v>
+      </c>
+      <c r="E286" s="19" t="s">
         <v>1104</v>
-      </c>
-      <c r="E286" s="19" t="s">
-        <v>1105</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="18" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B287" s="18" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C287" s="18" t="s">
         <v>305</v>
       </c>
       <c r="D287" s="20" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E287" s="20" t="s">
         <v>1106</v>
-      </c>
-      <c r="E287" s="20" t="s">
-        <v>1107</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="18" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B288" s="18" t="s">
         <v>304</v>
@@ -12350,10 +12346,10 @@
         <v>305</v>
       </c>
       <c r="D288" s="19" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E288" s="19" t="s">
         <v>1034</v>
-      </c>
-      <c r="E288" s="19" t="s">
-        <v>1035</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>